<commit_message>
backup: Pre-migration to Python BI-Engine - IntelligencePage with BubbleChart working
</commit_message>
<xml_diff>
--- a/data/vendedores.xlsx
+++ b/data/vendedores.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sistemas_ia\SalesMasters\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F5ED9C-EF61-4518-8C5F-E6421A4A9E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>VEN_CODIGO</t>
   </si>
@@ -87,57 +91,158 @@
     <t>GID</t>
   </si>
   <si>
-    <t>FABIOLA NANTES DE SOUZA</t>
-  </si>
-  <si>
-    <t>RUA EUGENIO DANERI, 181</t>
-  </si>
-  <si>
-    <t>CONJUNTO BURITI</t>
-  </si>
-  <si>
-    <t>CAMPO GRANDE</t>
-  </si>
-  <si>
-    <t>79091031</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>067-9176-4700</t>
-  </si>
-  <si>
-    <t>nds.fabiola@hotmail.com</t>
-  </si>
-  <si>
-    <t>FABIOLA NANTES</t>
-  </si>
-  <si>
-    <t>17/10</t>
-  </si>
-  <si>
-    <t>09C6AE6F-AA89-4988-BAC2-ED3DD021E1B2</t>
-  </si>
-  <si>
-    <t>PAOLA</t>
-  </si>
-  <si>
-    <t>DIRLEI OLIVEIRA</t>
-  </si>
-  <si>
-    <t>24/01</t>
+    <t>FABIO SILVA MASCARENHAS</t>
+  </si>
+  <si>
+    <t>RUA BARÃO DE MELGAÇO, 2754, SALA 303, 3º ANDAR</t>
+  </si>
+  <si>
+    <t>CENTRO SUL</t>
+  </si>
+  <si>
+    <t>CUIABÁ</t>
+  </si>
+  <si>
+    <t>78020-973</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>(65) 99607-1477</t>
+  </si>
+  <si>
+    <t>(65) 99607-1477</t>
+  </si>
+  <si>
+    <t>9162216615</t>
+  </si>
+  <si>
+    <t>fabio@targetrepresentacao.com.br</t>
+  </si>
+  <si>
+    <t>FABIO MASCARENHAS</t>
+  </si>
+  <si>
+    <t>01/01</t>
+  </si>
+  <si>
+    <t>25705205-7</t>
+  </si>
+  <si>
+    <t>GERENCIAL</t>
+  </si>
+  <si>
+    <t>(65) 99607-1477</t>
+  </si>
+  <si>
+    <t>ANGÉLICA CARVALHO</t>
+  </si>
+  <si>
+    <t>(65) 99610-7341</t>
+  </si>
+  <si>
+    <t>(65) 99610-7341</t>
+  </si>
+  <si>
+    <t>0000000000</t>
+  </si>
+  <si>
+    <t>JOSIELE ANDREIA</t>
+  </si>
+  <si>
+    <t>30/01</t>
+  </si>
+  <si>
+    <t>FABRICIO COSTA</t>
+  </si>
+  <si>
+    <t>(67) 99643 5091</t>
+  </si>
+  <si>
+    <t>(67) 98116 0071</t>
+  </si>
+  <si>
+    <t>aguirrerepresentacao@gmail.com</t>
+  </si>
+  <si>
+    <t>FABRICIO COSTA</t>
+  </si>
+  <si>
+    <t>01/01</t>
+  </si>
+  <si>
+    <t>DA23A221-4445-4B86-B742-40DB279267C7</t>
+  </si>
+  <si>
+    <t>SUPERVISÃO</t>
+  </si>
+  <si>
+    <t>(65) 99622-3373</t>
+  </si>
+  <si>
+    <t>BARBARA MOTTA</t>
+  </si>
+  <si>
+    <t>01/01</t>
+  </si>
+  <si>
+    <t>CAROLINA RIBEIRO</t>
+  </si>
+  <si>
+    <t>RUA PAVÃO, RECANTO SALVADOR</t>
+  </si>
+  <si>
+    <t>RECANTO DOS PASSAROS</t>
+  </si>
+  <si>
+    <t>CUIABA</t>
+  </si>
+  <si>
+    <t>78074118</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>(65) 99623-2987</t>
+  </si>
+  <si>
+    <t>(65) 99623-2987</t>
+  </si>
+  <si>
+    <t>02395241105</t>
+  </si>
+  <si>
+    <t>CAROLINA RIBEIRO</t>
+  </si>
+  <si>
+    <t>03/06</t>
+  </si>
+  <si>
+    <t>80E9E5C5-6363-47E7-AB56-4F747C2B5765</t>
+  </si>
+  <si>
+    <t>ANDREIA MASCARENHAS</t>
+  </si>
+  <si>
+    <t>(67) 99888-9884</t>
+  </si>
+  <si>
+    <t>ANDREIA MASCARENHAS</t>
+  </si>
+  <si>
+    <t>C4906152-AA88-47F3-8C04-92944B92118F</t>
+  </si>
+  <si>
+    <t>VENDEDOR NORTÃO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ [$R$]_-;\-* #,##0.00\ [$R$]_-;_-* &quot;-&quot;??\ [$R$]_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ [$R$]"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,14 +271,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -181,13 +281,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -225,7 +333,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -259,6 +367,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -293,9 +402,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -468,41 +578,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="8" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="150" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="60" customWidth="1"/>
     <col min="14" max="14" width="50" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
-    <col min="16" max="16" width="30" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
+    <col min="16" max="17" width="30" customWidth="1"/>
     <col min="18" max="18" width="100" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="20" max="21" width="12" customWidth="1"/>
     <col min="22" max="22" width="150" customWidth="1"/>
     <col min="23" max="23" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,8 +677,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -598,71 +702,205 @@
       <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="4">
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="7">
-        <v>2</v>
-      </c>
-      <c r="W2" t="s">
-        <v>33</v>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s">
+        <v>49</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>4</v>
+      </c>
+      <c r="W5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" s="7">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" s="2">
         <v>5</v>
+      </c>
+      <c r="W7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" t="s">
+        <v>69</v>
+      </c>
+      <c r="U8" s="2">
+        <v>6</v>
+      </c>
+      <c r="W8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
-    <oddFooter>&amp;LPage &amp;P of &amp;N
-</oddFooter>
+    <oddFooter>&amp;LPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: logo storage base64 and report fixes
</commit_message>
<xml_diff>
--- a/data/vendedores.xlsx
+++ b/data/vendedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sistemas_ia\SalesMasters\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6C9FEB-4056-40B0-A94A-B9754DA4A285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39149B64-44A1-4BFA-BB82-233DC5EF7A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>VEN_CODIGO</t>
   </si>
@@ -28,109 +28,34 @@
     <t>VEN_NOME</t>
   </si>
   <si>
-    <t>VEN_ENDERECO</t>
-  </si>
-  <si>
-    <t>VEN_BAIRRO</t>
-  </si>
-  <si>
-    <t>VEN_CIDADE</t>
-  </si>
-  <si>
-    <t>VEN_CEP</t>
-  </si>
-  <si>
-    <t>VEN_UF</t>
-  </si>
-  <si>
-    <t>VEN_FONE1</t>
-  </si>
-  <si>
-    <t>VEN_FONE2</t>
-  </si>
-  <si>
-    <t>VEN_OBS</t>
-  </si>
-  <si>
-    <t>VEN_CPF</t>
-  </si>
-  <si>
-    <t>VEN_COMISSAO</t>
-  </si>
-  <si>
-    <t>VEN_EMAIL</t>
-  </si>
-  <si>
-    <t>VEN_NOMEUSU</t>
-  </si>
-  <si>
-    <t>VEN_ANIVERSARIO</t>
-  </si>
-  <si>
-    <t>VEN_RG</t>
-  </si>
-  <si>
-    <t>VEN_CTPS</t>
-  </si>
-  <si>
-    <t>VEN_FILIACAO</t>
-  </si>
-  <si>
-    <t>VEN_PIS</t>
-  </si>
-  <si>
-    <t>VEN_FILHOS</t>
-  </si>
-  <si>
-    <t>VEN_CODUSU</t>
-  </si>
-  <si>
-    <t>VEN_IMAGEM</t>
-  </si>
-  <si>
-    <t>RODRIGO ODON</t>
-  </si>
-  <si>
-    <t>22/09</t>
-  </si>
-  <si>
-    <t>ANA RITA</t>
-  </si>
-  <si>
-    <t>RICARDO SCHAFIRSTEIN</t>
-  </si>
-  <si>
-    <t>KAILANNE MENDES DE NOVAIS</t>
-  </si>
-  <si>
-    <t>03/06</t>
-  </si>
-  <si>
-    <t>R.O CONSULT</t>
-  </si>
-  <si>
-    <t>MARIANA FREITAS</t>
-  </si>
-  <si>
-    <t>04/05</t>
-  </si>
-  <si>
-    <t>CAMILA ALMEIDA</t>
-  </si>
-  <si>
-    <t>30/04</t>
-  </si>
-  <si>
-    <t>JOÃO PEDRO</t>
-  </si>
-  <si>
-    <t>24/09</t>
-  </si>
-  <si>
-    <t>FERNANDA NOGUEIRA</t>
-  </si>
-  <si>
-    <t>26/11</t>
+    <t>MASTER</t>
+  </si>
+  <si>
+    <t>GRACIELA JANE PRADO</t>
+  </si>
+  <si>
+    <t>MARCELO AUGUSTO</t>
+  </si>
+  <si>
+    <t>ROGERIO LUIZ</t>
+  </si>
+  <si>
+    <t>PAULO HENRIQUE</t>
+  </si>
+  <si>
+    <t>JOÃO RICARDO</t>
+  </si>
+  <si>
+    <t>RICARDO MARCIO</t>
+  </si>
+  <si>
+    <t>MICHELLE FERREIRA MESQUITA</t>
+  </si>
+  <si>
+    <t>FABIO SOARES</t>
+  </si>
+  <si>
+    <t>ANA PAULA MONTEIRO</t>
   </si>
 </sst>
 </file>
@@ -473,217 +398,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="150" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="60" customWidth="1"/>
-    <col min="14" max="14" width="50" customWidth="1"/>
-    <col min="15" max="15" width="6" customWidth="1"/>
-    <col min="16" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="100" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="21" width="12" customWidth="1"/>
-    <col min="22" max="22" width="150" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="1">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>523</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="U6" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" t="s">
-        <v>30</v>
-      </c>
-      <c r="U7" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" t="s">
-        <v>32</v>
-      </c>
-      <c r="U8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>574</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" t="s">
-        <v>34</v>
-      </c>
-      <c r="U9" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <v>950</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="1">
-        <v>10</v>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1015</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Introduce a comprehensive set of new frontend components, backend endpoints, database scripts, BI engine modules, and agent-related files, alongside updates to the deployment script.
</commit_message>
<xml_diff>
--- a/data/vendedores.xlsx
+++ b/data/vendedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sistemas_ia\SalesMasters\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39149B64-44A1-4BFA-BB82-233DC5EF7A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685DF89C-D21D-4EAA-A892-E8F2AFDD3CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>VEN_CODIGO</t>
   </si>
@@ -28,34 +28,88 @@
     <t>VEN_NOME</t>
   </si>
   <si>
-    <t>MASTER</t>
-  </si>
-  <si>
-    <t>GRACIELA JANE PRADO</t>
-  </si>
-  <si>
-    <t>MARCELO AUGUSTO</t>
-  </si>
-  <si>
-    <t>ROGERIO LUIZ</t>
-  </si>
-  <si>
-    <t>PAULO HENRIQUE</t>
-  </si>
-  <si>
-    <t>JOÃO RICARDO</t>
-  </si>
-  <si>
-    <t>RICARDO MARCIO</t>
-  </si>
-  <si>
-    <t>MICHELLE FERREIRA MESQUITA</t>
-  </si>
-  <si>
-    <t>FABIO SOARES</t>
-  </si>
-  <si>
-    <t>ANA PAULA MONTEIRO</t>
+    <t>VEN_ENDERECO</t>
+  </si>
+  <si>
+    <t>VEN_BAIRRO</t>
+  </si>
+  <si>
+    <t>VEN_CIDADE</t>
+  </si>
+  <si>
+    <t>VEN_CEP</t>
+  </si>
+  <si>
+    <t>VEN_UF</t>
+  </si>
+  <si>
+    <t>VEN_FONE1</t>
+  </si>
+  <si>
+    <t>VEN_FONE2</t>
+  </si>
+  <si>
+    <t>VEN_OBS</t>
+  </si>
+  <si>
+    <t>VEN_CPF</t>
+  </si>
+  <si>
+    <t>VEN_COMISSAO</t>
+  </si>
+  <si>
+    <t>VEN_EMAIL</t>
+  </si>
+  <si>
+    <t>VEN_NOMEUSU</t>
+  </si>
+  <si>
+    <t>VEN_ANIVERSARIO</t>
+  </si>
+  <si>
+    <t>VEN_RG</t>
+  </si>
+  <si>
+    <t>VEN_CTPS</t>
+  </si>
+  <si>
+    <t>VEN_FILIACAO</t>
+  </si>
+  <si>
+    <t>VEN_PIS</t>
+  </si>
+  <si>
+    <t>VEN_FILHOS</t>
+  </si>
+  <si>
+    <t>VEN_CODUSU</t>
+  </si>
+  <si>
+    <t>VEN_IMAGEM</t>
+  </si>
+  <si>
+    <t>REMAP LTDA</t>
+  </si>
+  <si>
+    <t>SEBASTIÃO</t>
+  </si>
+  <si>
+    <t>PEDRO IVO</t>
+  </si>
+  <si>
+    <t>J CARLOS V. AÇO</t>
+  </si>
+  <si>
+    <t>J CARLOS ZM</t>
+  </si>
+  <si>
+    <t>J CARLOS</t>
+  </si>
+  <si>
+    <t>PEDRO FIUZA</t>
+  </si>
+  <si>
+    <t>J CARLOS ES</t>
   </si>
 </sst>
 </file>
@@ -398,102 +452,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="150" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="2" customWidth="1"/>
+    <col min="8" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="150" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="60" customWidth="1"/>
+    <col min="14" max="14" width="50" customWidth="1"/>
+    <col min="15" max="15" width="6" customWidth="1"/>
+    <col min="16" max="17" width="30" customWidth="1"/>
+    <col min="18" max="18" width="100" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>523</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>574</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>950</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1015</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>